<commit_message>
Uniandes 2023: pulir CV y terminar cursos y justificación
</commit_message>
<xml_diff>
--- a/Especial_Uniandes_2023/1. CV/data/education_es.xlsx
+++ b/Especial_Uniandes_2023/1. CV/data/education_es.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\Especial_Uniandes_2023\1. CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D03BD30-E451-4BE2-B990-EE19F355B74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D82BE-7A9B-4EAC-8384-FD8EC848D672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,12 +37,6 @@
     <t>why</t>
   </si>
   <si>
-    <t>PhD - Psychology</t>
-  </si>
-  <si>
-    <t>MSc in Evolutionary Psychology</t>
-  </si>
-  <si>
     <t>Stirling, Reino Unido</t>
   </si>
   <si>
@@ -80,6 +74,12 @@
   </si>
   <si>
     <t>Trabajo de Grado: 4.9/5.0</t>
+  </si>
+  <si>
+    <t>MSc in Evolutionary Psychology  \textit{(School of Biological Sciences)}</t>
+  </si>
+  <si>
+    <t>PhD - Psychology \textit{(\href{https://www.stir.ac.uk/about/faculties/natural-sciences/our-research/research-groups/behaviour-and-evolution-research-group/}{Behaviour and Evolution Research Group}, Faculty of Natural Sciences)}</t>
   </si>
 </sst>
 </file>
@@ -926,7 +926,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,21 +955,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1">
         <v>2014</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -987,24 +987,24 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>2009</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1013,24 +1013,24 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>2006</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>